<commit_message>
P-134 Ajout du test-bench de la DCT
</commit_message>
<xml_diff>
--- a/Code MFCC/DSK/MFCC_algorithme_pipeline_performance.xlsx
+++ b/Code MFCC/DSK/MFCC_algorithme_pipeline_performance.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t>fonction</t>
   </si>
@@ -35,6 +35,36 @@
   </si>
   <si>
     <t>FFT (DSPF_sp_cfftr4_dif)</t>
+  </si>
+  <si>
+    <t>FFT (DSPF_sp_cfftr2_dit)</t>
+  </si>
+  <si>
+    <t>freq2mel</t>
+  </si>
+  <si>
+    <t>mel2freq</t>
+  </si>
+  <si>
+    <t>MvgAvg</t>
+  </si>
+  <si>
+    <t>MelFilterBank Create</t>
+  </si>
+  <si>
+    <t>get MelCoeff</t>
+  </si>
+  <si>
+    <t>transfert between buffer 256</t>
+  </si>
+  <si>
+    <t>float2complex</t>
+  </si>
+  <si>
+    <t>FFT (DSPF_sp_cfftr2_dit) init</t>
+  </si>
+  <si>
+    <t>autocorrelation 256</t>
   </si>
 </sst>
 </file>
@@ -394,10 +424,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="C7:F10"/>
+  <dimension ref="C7:F32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -429,15 +459,15 @@
         <v>4</v>
       </c>
       <c r="D8" s="3">
-        <v>7853</v>
+        <v>7961</v>
       </c>
       <c r="E8" s="4">
         <f>D8/225000000*1000</f>
-        <v>3.4902222222222223E-2</v>
+        <v>3.5382222222222218E-2</v>
       </c>
       <c r="F8" s="5">
         <f>E8/10</f>
-        <v>3.4902222222222223E-3</v>
+        <v>3.5382222222222217E-3</v>
       </c>
     </row>
     <row r="9" spans="3:6" x14ac:dyDescent="0.25">
@@ -470,6 +500,176 @@
       <c r="F10" s="5">
         <f>E10/10</f>
         <v>1.6471111111111109E-3</v>
+      </c>
+    </row>
+    <row r="11" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C11" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D11" s="3">
+        <v>4839</v>
+      </c>
+      <c r="E11" s="4">
+        <f t="shared" ref="E11:E12" si="0">D11/225000000*1000</f>
+        <v>2.1506666666666664E-2</v>
+      </c>
+      <c r="F11" s="5">
+        <f t="shared" ref="F11:F12" si="1">E11/10</f>
+        <v>2.1506666666666662E-3</v>
+      </c>
+    </row>
+    <row r="12" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C12" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D12" s="3">
+        <v>98103</v>
+      </c>
+      <c r="E12" s="4">
+        <f t="shared" si="0"/>
+        <v>0.43601333333333331</v>
+      </c>
+      <c r="F12" s="5">
+        <f t="shared" si="1"/>
+        <v>4.3601333333333332E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C13" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D13" s="3">
+        <v>1646</v>
+      </c>
+      <c r="E13" s="4">
+        <f>D13/225000000*1000</f>
+        <v>7.315555555555556E-3</v>
+      </c>
+      <c r="F13" s="5">
+        <f>E13/10</f>
+        <v>7.315555555555556E-4</v>
+      </c>
+    </row>
+    <row r="14" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C14" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D14" s="3">
+        <v>1278</v>
+      </c>
+      <c r="E14" s="4">
+        <f>D14/225000000*1000</f>
+        <v>5.6800000000000002E-3</v>
+      </c>
+      <c r="F14" s="5">
+        <f>E14/10</f>
+        <v>5.6800000000000004E-4</v>
+      </c>
+    </row>
+    <row r="15" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C15" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D15" s="3">
+        <v>253</v>
+      </c>
+      <c r="E15" s="4">
+        <f>D15/225000000*1000</f>
+        <v>1.1244444444444444E-3</v>
+      </c>
+      <c r="F15" s="5">
+        <f>E15/10</f>
+        <v>1.1244444444444445E-4</v>
+      </c>
+    </row>
+    <row r="16" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C16" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D16" s="3">
+        <v>323319</v>
+      </c>
+      <c r="E16" s="4">
+        <f>D16/225000000*1000</f>
+        <v>1.4369733333333334</v>
+      </c>
+      <c r="F16" s="5">
+        <f>E16/10</f>
+        <v>0.14369733333333334</v>
+      </c>
+    </row>
+    <row r="17" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C17" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D17" s="3">
+        <v>12225</v>
+      </c>
+      <c r="E17" s="4">
+        <f>D17/225000000*1000</f>
+        <v>5.4333333333333331E-2</v>
+      </c>
+      <c r="F17" s="5">
+        <f>E17/10</f>
+        <v>5.4333333333333334E-3</v>
+      </c>
+    </row>
+    <row r="18" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C18" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D18" s="3">
+        <v>6154</v>
+      </c>
+      <c r="E18" s="4">
+        <f>D18/225000000*1000</f>
+        <v>2.7351111111111111E-2</v>
+      </c>
+      <c r="F18" s="5">
+        <f>E18/10</f>
+        <v>2.7351111111111109E-3</v>
+      </c>
+    </row>
+    <row r="19" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C19" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D19" s="3">
+        <v>16169</v>
+      </c>
+      <c r="E19" s="4">
+        <f>D19/225000000*1000</f>
+        <v>7.1862222222222216E-2</v>
+      </c>
+      <c r="F19" s="5">
+        <f>E19/10</f>
+        <v>7.1862222222222214E-3</v>
+      </c>
+    </row>
+    <row r="20" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C20" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D20" s="3">
+        <v>203980</v>
+      </c>
+      <c r="E20" s="4">
+        <f>D20/225000000*1000</f>
+        <v>0.90657777777777782</v>
+      </c>
+      <c r="F20" s="5">
+        <f>E20/10</f>
+        <v>9.0657777777777782E-2</v>
+      </c>
+    </row>
+    <row r="21" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="E21" s="4"/>
+      <c r="F21" s="5"/>
+    </row>
+    <row r="32" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="F32" s="5">
+        <f>SUM(F8:F31)</f>
+        <v>0.30428622222222224</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
P-122 nouvelle structure simple pour l'algo MFCC
</commit_message>
<xml_diff>
--- a/Code MFCC/DSK/MFCC_algorithme_pipeline_performance.xlsx
+++ b/Code MFCC/DSK/MFCC_algorithme_pipeline_performance.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="21">
   <si>
     <t>fonction</t>
   </si>
@@ -65,6 +65,18 @@
   </si>
   <si>
     <t>autocorrelation 256</t>
+  </si>
+  <si>
+    <t>DCT 20 - &gt; 20 coeffs</t>
+  </si>
+  <si>
+    <t>DCT init</t>
+  </si>
+  <si>
+    <t>run</t>
+  </si>
+  <si>
+    <t>init</t>
   </si>
 </sst>
 </file>
@@ -424,10 +436,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="C7:F32"/>
+  <dimension ref="C6:G31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="D23" sqref="D23"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="G25" sqref="G25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -436,11 +448,19 @@
     <col min="3" max="3" width="45.85546875" style="3" customWidth="1"/>
     <col min="4" max="4" width="16.85546875" style="3" customWidth="1"/>
     <col min="5" max="5" width="21.140625" style="3" customWidth="1"/>
-    <col min="6" max="6" width="12.7109375" style="3" customWidth="1"/>
-    <col min="7" max="16384" width="9.140625" style="3"/>
+    <col min="6" max="7" width="12.7109375" style="3" customWidth="1"/>
+    <col min="8" max="16384" width="9.140625" style="3"/>
   </cols>
   <sheetData>
-    <row r="7" spans="3:6" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="F6" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="G6" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="7" spans="3:7" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C7" s="1" t="s">
         <v>0</v>
       </c>
@@ -453,8 +473,11 @@
       <c r="F7" s="2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="8" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="G7" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C8" s="3" t="s">
         <v>4</v>
       </c>
@@ -465,12 +488,9 @@
         <f>D8/225000000*1000</f>
         <v>3.5382222222222218E-2</v>
       </c>
-      <c r="F8" s="5">
-        <f>E8/10</f>
-        <v>3.5382222222222217E-3</v>
-      </c>
-    </row>
-    <row r="9" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="F8" s="5"/>
+    </row>
+    <row r="9" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C9" s="3" t="s">
         <v>5</v>
       </c>
@@ -481,12 +501,9 @@
         <f>D9/225000000*1000</f>
         <v>2.227111111111111E-2</v>
       </c>
-      <c r="F9" s="5">
-        <f>E9/10</f>
-        <v>2.2271111111111111E-3</v>
-      </c>
-    </row>
-    <row r="10" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="F9" s="5"/>
+    </row>
+    <row r="10" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C10" s="3" t="s">
         <v>6</v>
       </c>
@@ -502,7 +519,7 @@
         <v>1.6471111111111109E-3</v>
       </c>
     </row>
-    <row r="11" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C11" s="3" t="s">
         <v>7</v>
       </c>
@@ -518,7 +535,7 @@
         <v>2.1506666666666662E-3</v>
       </c>
     </row>
-    <row r="12" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C12" s="3" t="s">
         <v>15</v>
       </c>
@@ -529,12 +546,12 @@
         <f t="shared" si="0"/>
         <v>0.43601333333333331</v>
       </c>
-      <c r="F12" s="5">
-        <f t="shared" si="1"/>
+      <c r="G12" s="5">
+        <f>E12/10</f>
         <v>4.3601333333333332E-2</v>
       </c>
     </row>
-    <row r="13" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C13" s="3" t="s">
         <v>8</v>
       </c>
@@ -542,15 +559,15 @@
         <v>1646</v>
       </c>
       <c r="E13" s="4">
-        <f>D13/225000000*1000</f>
+        <f t="shared" ref="E13:E31" si="2">D13/225000000*1000</f>
         <v>7.315555555555556E-3</v>
       </c>
       <c r="F13" s="5">
-        <f>E13/10</f>
+        <f t="shared" ref="F13:F31" si="3">E13/10</f>
         <v>7.315555555555556E-4</v>
       </c>
     </row>
-    <row r="14" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C14" s="3" t="s">
         <v>9</v>
       </c>
@@ -558,15 +575,15 @@
         <v>1278</v>
       </c>
       <c r="E14" s="4">
-        <f>D14/225000000*1000</f>
+        <f t="shared" si="2"/>
         <v>5.6800000000000002E-3</v>
       </c>
       <c r="F14" s="5">
-        <f>E14/10</f>
+        <f t="shared" si="3"/>
         <v>5.6800000000000004E-4</v>
       </c>
     </row>
-    <row r="15" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C15" s="3" t="s">
         <v>10</v>
       </c>
@@ -574,15 +591,15 @@
         <v>253</v>
       </c>
       <c r="E15" s="4">
-        <f>D15/225000000*1000</f>
+        <f t="shared" si="2"/>
         <v>1.1244444444444444E-3</v>
       </c>
       <c r="F15" s="5">
-        <f>E15/10</f>
+        <f t="shared" si="3"/>
         <v>1.1244444444444445E-4</v>
       </c>
     </row>
-    <row r="16" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C16" s="3" t="s">
         <v>11</v>
       </c>
@@ -590,15 +607,15 @@
         <v>323319</v>
       </c>
       <c r="E16" s="4">
-        <f>D16/225000000*1000</f>
+        <f t="shared" si="2"/>
         <v>1.4369733333333334</v>
       </c>
-      <c r="F16" s="5">
+      <c r="G16" s="5">
         <f>E16/10</f>
         <v>0.14369733333333334</v>
       </c>
     </row>
-    <row r="17" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C17" s="3" t="s">
         <v>12</v>
       </c>
@@ -606,15 +623,15 @@
         <v>12225</v>
       </c>
       <c r="E17" s="4">
-        <f>D17/225000000*1000</f>
+        <f t="shared" si="2"/>
         <v>5.4333333333333331E-2</v>
       </c>
       <c r="F17" s="5">
-        <f>E17/10</f>
+        <f t="shared" si="3"/>
         <v>5.4333333333333334E-3</v>
       </c>
     </row>
-    <row r="18" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C18" s="3" t="s">
         <v>13</v>
       </c>
@@ -622,15 +639,15 @@
         <v>6154</v>
       </c>
       <c r="E18" s="4">
-        <f>D18/225000000*1000</f>
+        <f t="shared" si="2"/>
         <v>2.7351111111111111E-2</v>
       </c>
       <c r="F18" s="5">
-        <f>E18/10</f>
+        <f t="shared" si="3"/>
         <v>2.7351111111111109E-3</v>
       </c>
     </row>
-    <row r="19" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C19" s="3" t="s">
         <v>14</v>
       </c>
@@ -638,15 +655,15 @@
         <v>16169</v>
       </c>
       <c r="E19" s="4">
-        <f>D19/225000000*1000</f>
+        <f t="shared" si="2"/>
         <v>7.1862222222222216E-2</v>
       </c>
       <c r="F19" s="5">
-        <f>E19/10</f>
+        <f t="shared" si="3"/>
         <v>7.1862222222222214E-3</v>
       </c>
     </row>
-    <row r="20" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C20" s="3" t="s">
         <v>16</v>
       </c>
@@ -654,23 +671,83 @@
         <v>203980</v>
       </c>
       <c r="E20" s="4">
-        <f>D20/225000000*1000</f>
+        <f t="shared" si="2"/>
         <v>0.90657777777777782</v>
       </c>
       <c r="F20" s="5">
-        <f>E20/10</f>
+        <f t="shared" si="3"/>
         <v>9.0657777777777782E-2</v>
       </c>
     </row>
-    <row r="21" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="E21" s="4"/>
-      <c r="F21" s="5"/>
-    </row>
-    <row r="32" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="F32" s="5">
-        <f>SUM(F8:F31)</f>
-        <v>0.30428622222222224</v>
-      </c>
+    <row r="21" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C21" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D21" s="3">
+        <v>324781</v>
+      </c>
+      <c r="E21" s="4">
+        <f t="shared" si="2"/>
+        <v>1.4434711111111111</v>
+      </c>
+      <c r="G21" s="5">
+        <f>E21/10</f>
+        <v>0.14434711111111112</v>
+      </c>
+    </row>
+    <row r="22" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C22" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D22" s="3">
+        <v>20834</v>
+      </c>
+      <c r="E22" s="4">
+        <f t="shared" si="2"/>
+        <v>9.2595555555555556E-2</v>
+      </c>
+      <c r="F22" s="5">
+        <f t="shared" si="3"/>
+        <v>9.2595555555555556E-3</v>
+      </c>
+    </row>
+    <row r="23" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="E23" s="4"/>
+      <c r="F23" s="5"/>
+    </row>
+    <row r="24" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="E24" s="4"/>
+      <c r="F24" s="5"/>
+    </row>
+    <row r="25" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="E25" s="4"/>
+      <c r="F25" s="5">
+        <f ca="1">SUM(F8:F31)</f>
+        <v>0.12048177777777777</v>
+      </c>
+    </row>
+    <row r="26" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="E26" s="4"/>
+    </row>
+    <row r="27" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="E27" s="4"/>
+      <c r="F27" s="5"/>
+    </row>
+    <row r="28" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="E28" s="4"/>
+      <c r="F28" s="5"/>
+    </row>
+    <row r="29" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="E29" s="4"/>
+      <c r="F29" s="5"/>
+    </row>
+    <row r="30" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="E30" s="4"/>
+      <c r="F30" s="5"/>
+    </row>
+    <row r="31" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="E31" s="4"/>
+      <c r="F31" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
P-197 Ajout des fichier .c et .h dans le répertoire CCS
dsk.h/dsk.c
wave.h/wave.c
</commit_message>
<xml_diff>
--- a/Code MFCC/DSK/MFCC_algorithme_pipeline_performance.xlsx
+++ b/Code MFCC/DSK/MFCC_algorithme_pipeline_performance.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="22">
   <si>
     <t>fonction</t>
   </si>
@@ -77,6 +77,9 @@
   </si>
   <si>
     <t>init</t>
+  </si>
+  <si>
+    <t>Pipeline MFCC 13 coefficient (256 donné)</t>
   </si>
 </sst>
 </file>
@@ -438,8 +441,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C6:G31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="G25" sqref="G25"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -488,7 +491,10 @@
         <f>D8/225000000*1000</f>
         <v>3.5382222222222218E-2</v>
       </c>
-      <c r="F8" s="5"/>
+      <c r="F8" s="5">
+        <f t="shared" ref="F8:F9" si="0">E8/10</f>
+        <v>3.5382222222222217E-3</v>
+      </c>
     </row>
     <row r="9" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C9" s="3" t="s">
@@ -501,7 +507,10 @@
         <f>D9/225000000*1000</f>
         <v>2.227111111111111E-2</v>
       </c>
-      <c r="F9" s="5"/>
+      <c r="F9" s="5">
+        <f t="shared" si="0"/>
+        <v>2.2271111111111111E-3</v>
+      </c>
     </row>
     <row r="10" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C10" s="3" t="s">
@@ -527,11 +536,11 @@
         <v>4839</v>
       </c>
       <c r="E11" s="4">
-        <f t="shared" ref="E11:E12" si="0">D11/225000000*1000</f>
+        <f t="shared" ref="E11:E12" si="1">D11/225000000*1000</f>
         <v>2.1506666666666664E-2</v>
       </c>
       <c r="F11" s="5">
-        <f t="shared" ref="F11:F12" si="1">E11/10</f>
+        <f t="shared" ref="F11" si="2">E11/10</f>
         <v>2.1506666666666662E-3</v>
       </c>
     </row>
@@ -543,10 +552,10 @@
         <v>98103</v>
       </c>
       <c r="E12" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.43601333333333331</v>
       </c>
-      <c r="G12" s="5">
+      <c r="F12" s="5">
         <f>E12/10</f>
         <v>4.3601333333333332E-2</v>
       </c>
@@ -559,11 +568,11 @@
         <v>1646</v>
       </c>
       <c r="E13" s="4">
-        <f t="shared" ref="E13:E31" si="2">D13/225000000*1000</f>
+        <f t="shared" ref="E13:E22" si="3">D13/225000000*1000</f>
         <v>7.315555555555556E-3</v>
       </c>
       <c r="F13" s="5">
-        <f t="shared" ref="F13:F31" si="3">E13/10</f>
+        <f t="shared" ref="F13:F22" si="4">E13/10</f>
         <v>7.315555555555556E-4</v>
       </c>
     </row>
@@ -575,11 +584,11 @@
         <v>1278</v>
       </c>
       <c r="E14" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>5.6800000000000002E-3</v>
       </c>
       <c r="F14" s="5">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>5.6800000000000004E-4</v>
       </c>
     </row>
@@ -591,11 +600,11 @@
         <v>253</v>
       </c>
       <c r="E15" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1.1244444444444444E-3</v>
       </c>
       <c r="F15" s="5">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>1.1244444444444445E-4</v>
       </c>
     </row>
@@ -607,15 +616,15 @@
         <v>323319</v>
       </c>
       <c r="E16" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1.4369733333333334</v>
       </c>
-      <c r="G16" s="5">
+      <c r="F16" s="5">
         <f>E16/10</f>
         <v>0.14369733333333334</v>
       </c>
     </row>
-    <row r="17" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C17" s="3" t="s">
         <v>12</v>
       </c>
@@ -623,15 +632,15 @@
         <v>12225</v>
       </c>
       <c r="E17" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>5.4333333333333331E-2</v>
       </c>
       <c r="F17" s="5">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>5.4333333333333334E-3</v>
       </c>
     </row>
-    <row r="18" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C18" s="3" t="s">
         <v>13</v>
       </c>
@@ -639,15 +648,15 @@
         <v>6154</v>
       </c>
       <c r="E18" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>2.7351111111111111E-2</v>
       </c>
       <c r="F18" s="5">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>2.7351111111111109E-3</v>
       </c>
     </row>
-    <row r="19" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C19" s="3" t="s">
         <v>14</v>
       </c>
@@ -655,15 +664,15 @@
         <v>16169</v>
       </c>
       <c r="E19" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>7.1862222222222216E-2</v>
       </c>
       <c r="F19" s="5">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>7.1862222222222214E-3</v>
       </c>
     </row>
-    <row r="20" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="20" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C20" s="3" t="s">
         <v>16</v>
       </c>
@@ -671,15 +680,15 @@
         <v>203980</v>
       </c>
       <c r="E20" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.90657777777777782</v>
       </c>
       <c r="F20" s="5">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>9.0657777777777782E-2</v>
       </c>
     </row>
-    <row r="21" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="21" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C21" s="3" t="s">
         <v>18</v>
       </c>
@@ -687,15 +696,15 @@
         <v>324781</v>
       </c>
       <c r="E21" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1.4434711111111111</v>
       </c>
-      <c r="G21" s="5">
+      <c r="F21" s="5">
         <f>E21/10</f>
         <v>0.14434711111111112</v>
       </c>
     </row>
-    <row r="22" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="22" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C22" s="3" t="s">
         <v>17</v>
       </c>
@@ -703,49 +712,61 @@
         <v>20834</v>
       </c>
       <c r="E22" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>9.2595555555555556E-2</v>
       </c>
       <c r="F22" s="5">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>9.2595555555555556E-3</v>
       </c>
     </row>
-    <row r="23" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="23" spans="3:6" x14ac:dyDescent="0.25">
       <c r="E23" s="4"/>
-      <c r="F23" s="5"/>
-    </row>
-    <row r="24" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="F23" s="5">
+        <f>SUM(F8:F22)</f>
+        <v>0.4578928888888889</v>
+      </c>
+    </row>
+    <row r="24" spans="3:6" x14ac:dyDescent="0.25">
       <c r="E24" s="4"/>
       <c r="F24" s="5"/>
     </row>
-    <row r="25" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="E25" s="4"/>
+    <row r="25" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C25" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="D25" s="3">
+        <v>78783</v>
+      </c>
+      <c r="E25" s="4">
+        <f t="shared" ref="E25" si="5">D25/225000000*1000</f>
+        <v>0.35014666666666666</v>
+      </c>
       <c r="F25" s="5">
-        <f ca="1">SUM(F8:F31)</f>
-        <v>0.12048177777777777</v>
-      </c>
-    </row>
-    <row r="26" spans="3:7" x14ac:dyDescent="0.25">
+        <f t="shared" ref="F25" si="6">E25/10</f>
+        <v>3.5014666666666666E-2</v>
+      </c>
+    </row>
+    <row r="26" spans="3:6" x14ac:dyDescent="0.25">
       <c r="E26" s="4"/>
     </row>
-    <row r="27" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="27" spans="3:6" x14ac:dyDescent="0.25">
       <c r="E27" s="4"/>
       <c r="F27" s="5"/>
     </row>
-    <row r="28" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="28" spans="3:6" x14ac:dyDescent="0.25">
       <c r="E28" s="4"/>
       <c r="F28" s="5"/>
     </row>
-    <row r="29" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="29" spans="3:6" x14ac:dyDescent="0.25">
       <c r="E29" s="4"/>
       <c r="F29" s="5"/>
     </row>
-    <row r="30" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="30" spans="3:6" x14ac:dyDescent="0.25">
       <c r="E30" s="4"/>
       <c r="F30" s="5"/>
     </row>
-    <row r="31" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="31" spans="3:6" x14ac:dyDescent="0.25">
       <c r="E31" s="4"/>
       <c r="F31" s="5"/>
     </row>

</xml_diff>

<commit_message>
Fonction de construction de dictionnaire fonctionnelle
</commit_message>
<xml_diff>
--- a/Code MFCC/DSK/MFCC_algorithme_pipeline_performance.xlsx
+++ b/Code MFCC/DSK/MFCC_algorithme_pipeline_performance.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="23">
   <si>
     <t>fonction</t>
   </si>
@@ -80,6 +80,9 @@
   </si>
   <si>
     <t>Pipeline MFCC 13 coefficient (256 donné)</t>
+  </si>
+  <si>
+    <t>CB construction (2000 sample, 16 CW)</t>
   </si>
 </sst>
 </file>
@@ -118,7 +121,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -133,6 +136,9 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -442,7 +448,7 @@
   <dimension ref="C6:G31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D24" sqref="D24"/>
+      <selection activeCell="C31" sqref="C31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -748,7 +754,20 @@
       </c>
     </row>
     <row r="26" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="E26" s="4"/>
+      <c r="C26" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D26" s="6">
+        <v>456541351</v>
+      </c>
+      <c r="E26" s="4">
+        <f t="shared" ref="E26" si="7">D26/225000000*1000</f>
+        <v>2029.0726711111108</v>
+      </c>
+      <c r="F26" s="5">
+        <f t="shared" ref="F26" si="8">E26/10</f>
+        <v>202.90726711111108</v>
+      </c>
     </row>
     <row r="27" spans="3:6" x14ac:dyDescent="0.25">
       <c r="E27" s="4"/>

</xml_diff>